<commit_message>
Added some more to Work Plan
In other comitments
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -26,8 +26,41 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Benjamin Joshua Charlton</author>
+  </authors>
+  <commentList>
+    <comment ref="A23" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Benjamin Joshua Charlton:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Not counting in revision time 
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Week</t>
   </si>
@@ -67,13 +100,19 @@
   </si>
   <si>
     <t>Other Commitments</t>
+  </si>
+  <si>
+    <t>Welcome Week</t>
+  </si>
+  <si>
+    <t>Autumn Exams</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -89,13 +128,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -139,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="180" wrapText="1"/>
@@ -151,6 +207,8 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,19 +485,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
     <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="6.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.5" customWidth="1"/>
@@ -574,7 +632,7 @@
       <c r="AH2" s="3"/>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -588,7 +646,7 @@
       <c r="A6" s="6"/>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -605,7 +663,7 @@
       <c r="A11" s="6"/>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="8" t="s">
         <v>8</v>
       </c>
     </row>
@@ -621,56 +679,63 @@
     <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="6"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="7"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
@@ -684,5 +749,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made brief notes on Work Plan
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Week</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>Autumn Exams</t>
+  </si>
+  <si>
+    <t>Project Proposal</t>
+  </si>
+  <si>
+    <t>15 December - 15 January Christmas</t>
+  </si>
+  <si>
+    <t>23 March - 23 April Easter</t>
   </si>
 </sst>
 </file>
@@ -140,7 +149,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,7 +158,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -195,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="180" wrapText="1"/>
@@ -207,8 +222,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,7 +508,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -632,12 +648,16 @@
       <c r="AH2" s="3"/>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
+      <c r="A4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
@@ -646,7 +666,7 @@
       <c r="A6" s="6"/>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
     </row>
@@ -663,7 +683,7 @@
       <c r="A11" s="6"/>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -680,7 +700,7 @@
       <c r="A16" s="6"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -694,7 +714,7 @@
       <c r="A20" s="6"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="7" t="s">
         <v>11</v>
       </c>
     </row>
@@ -702,14 +722,14 @@
       <c r="A22" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="7"/>
+      <c r="B22" s="9"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="R23" s="7"/>
-      <c r="S23" s="7"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
@@ -719,9 +739,15 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
+      <c r="H26" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
+      <c r="H27" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>

</xml_diff>

<commit_message>
Created list in proposal for work plan
This section is detailing all of the sections in the work plan gantt chart
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="440" windowWidth="22900" windowHeight="28360" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="440" windowWidth="40880" windowHeight="25160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <author>Benjamin Joshua Charlton</author>
   </authors>
   <commentList>
-    <comment ref="A23" authorId="0">
+    <comment ref="A24" authorId="0">
       <text>
         <r>
           <rPr>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Week</t>
   </si>
@@ -111,10 +111,25 @@
     <t>Project Proposal</t>
   </si>
   <si>
-    <t>15 December - 15 January Christmas</t>
-  </si>
-  <si>
-    <t>23 March - 23 April Easter</t>
+    <t>Christmas Holiday</t>
+  </si>
+  <si>
+    <t>Easter Holiday</t>
+  </si>
+  <si>
+    <t>Dissertation</t>
+  </si>
+  <si>
+    <t>Interrim Report</t>
+  </si>
+  <si>
+    <t>Create GA Structure</t>
+  </si>
+  <si>
+    <t>Install relevant libaries</t>
+  </si>
+  <si>
+    <t>GA Structure and libaries happen hand in hand 1 week</t>
   </si>
 </sst>
 </file>
@@ -210,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="180" wrapText="1"/>
@@ -225,6 +240,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,13 +518,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH35"/>
+  <dimension ref="A1:AH36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H28" sqref="H28"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -660,10 +676,20 @@
       <c r="D4" s="8"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
+      <c r="A5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
+      <c r="A6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB6" s="8"/>
+      <c r="AC6" s="8"/>
+      <c r="AD6" s="8"/>
+      <c r="AE6" s="8"/>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
@@ -688,7 +714,9 @@
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
+      <c r="A13" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14" s="6"/>
@@ -699,79 +727,94 @@
     <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B22" s="9"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="10"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="R23" s="9"/>
-      <c r="S23" s="9"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A24" s="6"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A25" s="6"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB25" s="9"/>
+      <c r="AC25" s="9"/>
+      <c r="AD25" s="9"/>
+      <c r="AE25" s="9"/>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
-      <c r="H26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
-      <c r="H27" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="H33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added more to work plan
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -32,7 +32,7 @@
     <author>Benjamin Joshua Charlton</author>
   </authors>
   <commentList>
-    <comment ref="A24" authorId="0">
+    <comment ref="A25" authorId="0">
       <text>
         <r>
           <rPr>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Week</t>
   </si>
@@ -126,10 +126,17 @@
     <t>Create GA Structure</t>
   </si>
   <si>
-    <t>Install relevant libaries</t>
-  </si>
-  <si>
     <t>GA Structure and libaries happen hand in hand 1 week</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23rd October
+Revised Project Proposal </t>
+  </si>
+  <si>
+    <t>Revised Project Proposal</t>
+  </si>
+  <si>
+    <t>Install software</t>
   </si>
 </sst>
 </file>
@@ -518,13 +525,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH36"/>
+  <dimension ref="A1:AH37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -541,7 +548,7 @@
     <col min="29" max="33" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="1" customFormat="1" ht="106" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" s="1" customFormat="1" ht="127" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -550,6 +557,9 @@
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>5</v>
@@ -677,27 +687,32 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
+        <v>22</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="AB6" s="8"/>
-      <c r="AC6" s="8"/>
-      <c r="AD6" s="8"/>
-      <c r="AE6" s="8"/>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="AB7" s="8"/>
+      <c r="AC7" s="8"/>
+      <c r="AD7" s="8"/>
+      <c r="AE7" s="8"/>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
@@ -709,17 +724,17 @@
       <c r="A11" s="6"/>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6"/>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
@@ -728,60 +743,60 @@
       <c r="A16" s="6"/>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6"/>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
+      <c r="A19" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6"/>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="9"/>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="10"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
+        <v>12</v>
+      </c>
+      <c r="B23" s="9"/>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="R24" s="9"/>
-      <c r="S24" s="9"/>
+        <v>15</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="AB25" s="9"/>
-      <c r="AC25" s="9"/>
-      <c r="AD25" s="9"/>
-      <c r="AE25" s="9"/>
-    </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A26" s="6"/>
+      <c r="AB26" s="9"/>
+      <c r="AC26" s="9"/>
+      <c r="AD26" s="9"/>
+      <c r="AE26" s="9"/>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
@@ -803,18 +818,21 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
-      <c r="H33" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>
+      <c r="H34" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="6"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Further Updates to work plan
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Week</t>
   </si>
@@ -126,9 +126,6 @@
     <t>Create GA Structure</t>
   </si>
   <si>
-    <t>GA Structure and libaries happen hand in hand 1 week</t>
-  </si>
-  <si>
     <t xml:space="preserve">23rd October
 Revised Project Proposal </t>
   </si>
@@ -137,6 +134,12 @@
   </si>
   <si>
     <t>Install software</t>
+  </si>
+  <si>
+    <t>Review languages for Eas</t>
+  </si>
+  <si>
+    <t>Research EAs</t>
   </si>
 </sst>
 </file>
@@ -171,7 +174,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,6 +190,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -232,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="180" wrapText="1"/>
@@ -248,6 +269,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,12 +555,12 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="6.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.5" customWidth="1"/>
@@ -559,7 +583,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>5</v>
@@ -687,7 +711,7 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -715,10 +739,16 @@
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
+      <c r="A9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
+      <c r="A10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
@@ -735,6 +765,7 @@
       <c r="A14" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
@@ -752,8 +783,10 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>23</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
@@ -816,22 +849,19 @@
     <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>
-      <c r="H34" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="6"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work Plan completed? till christmas
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -32,7 +32,7 @@
     <author>Benjamin Joshua Charlton</author>
   </authors>
   <commentList>
-    <comment ref="A25" authorId="0">
+    <comment ref="A27" authorId="0">
       <text>
         <r>
           <rPr>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Week</t>
   </si>
@@ -140,6 +140,24 @@
   </si>
   <si>
     <t>Research EAs</t>
+  </si>
+  <si>
+    <t>Research Representation</t>
+  </si>
+  <si>
+    <t>Representation</t>
+  </si>
+  <si>
+    <t>Basic Methods for GA</t>
+  </si>
+  <si>
+    <t>Data import</t>
+  </si>
+  <si>
+    <t>Validation Method</t>
+  </si>
+  <si>
+    <t>Needs a slot</t>
   </si>
 </sst>
 </file>
@@ -549,13 +567,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH37"/>
+  <dimension ref="A1:AH39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -751,7 +769,10 @@
       <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
+      <c r="A11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
@@ -768,74 +789,96 @@
       <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
+      <c r="A15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
+      <c r="A16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="10"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
+      <c r="A17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A19" s="6"/>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-    </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-    </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6"/>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A23" s="6"/>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="9"/>
-    </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="10"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="R25" s="9"/>
-      <c r="S25" s="9"/>
+        <v>12</v>
+      </c>
+      <c r="B25" s="9"/>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="10"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="AB26" s="9"/>
-      <c r="AC26" s="9"/>
-      <c r="AD26" s="9"/>
-      <c r="AE26" s="9"/>
-    </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A27" s="6"/>
-    </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A28" s="6"/>
+      <c r="AB28" s="9"/>
+      <c r="AC28" s="9"/>
+      <c r="AD28" s="9"/>
+      <c r="AE28" s="9"/>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
@@ -863,6 +906,12 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="6"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updates to work plan and references
Final commit of this work session
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Week</t>
   </si>
@@ -155,9 +155,6 @@
   </si>
   <si>
     <t>Validation Method</t>
-  </si>
-  <si>
-    <t>Needs a slot</t>
   </si>
 </sst>
 </file>
@@ -573,7 +570,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomRight" activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -816,11 +813,11 @@
       <c r="A18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B18" t="s">
-        <v>30</v>
-      </c>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>

</xml_diff>

<commit_message>
Updated Workplan after Interim report
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="440" windowWidth="40880" windowHeight="25160" tabRatio="500"/>
+    <workbookView xWindow="5240" yWindow="-21160" windowWidth="38400" windowHeight="21160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <author>Benjamin Joshua Charlton</author>
   </authors>
   <commentList>
-    <comment ref="A27" authorId="0">
+    <comment ref="A29" authorId="0">
       <text>
         <r>
           <rPr>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Week</t>
   </si>
@@ -155,6 +155,18 @@
   </si>
   <si>
     <t>Validation Method</t>
+  </si>
+  <si>
+    <t>Run Basic Methods</t>
+  </si>
+  <si>
+    <t>Research advanced EA methods</t>
+  </si>
+  <si>
+    <t>Advanced Methods for GA</t>
+  </si>
+  <si>
+    <t>Bug Fixing 1</t>
   </si>
 </sst>
 </file>
@@ -268,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="180" wrapText="1"/>
@@ -287,6 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,13 +577,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH39"/>
+  <dimension ref="A1:AH41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O8" sqref="O8"/>
+      <selection pane="bottomRight" activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -772,7 +785,13 @@
       <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
+      <c r="A12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
@@ -817,71 +836,97 @@
       <c r="K18" s="10"/>
       <c r="M18" s="11"/>
       <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
+      <c r="O18" s="10"/>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
+      <c r="A19" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A21" s="6"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-    </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
-    </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A23" s="6"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A25" s="6"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="9"/>
-    </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" s="10"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="9"/>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="R27" s="9"/>
-      <c r="S27" s="9"/>
+        <v>12</v>
+      </c>
+      <c r="B27" s="9"/>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="10"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="AB28" s="9"/>
-      <c r="AC28" s="9"/>
-      <c r="AD28" s="9"/>
-      <c r="AE28" s="9"/>
-    </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A29" s="6"/>
-    </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A30" s="6"/>
+      <c r="AB30" s="9"/>
+      <c r="AC30" s="9"/>
+      <c r="AD30" s="9"/>
+      <c r="AE30" s="9"/>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
@@ -909,6 +954,12 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="6"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
First Draft of work plan
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -32,7 +32,7 @@
     <author>Benjamin Joshua Charlton</author>
   </authors>
   <commentList>
-    <comment ref="A29" authorId="0">
+    <comment ref="A31" authorId="0">
       <text>
         <r>
           <rPr>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>Week</t>
   </si>
@@ -136,15 +136,6 @@
     <t>Install software</t>
   </si>
   <si>
-    <t>Review languages for Eas</t>
-  </si>
-  <si>
-    <t>Research EAs</t>
-  </si>
-  <si>
-    <t>Research Representation</t>
-  </si>
-  <si>
     <t>Representation</t>
   </si>
   <si>
@@ -160,13 +151,31 @@
     <t>Run Basic Methods</t>
   </si>
   <si>
-    <t>Research advanced EA methods</t>
-  </si>
-  <si>
     <t>Advanced Methods for GA</t>
   </si>
   <si>
     <t>Bug Fixing 1</t>
+  </si>
+  <si>
+    <t>Advanced EA methods</t>
+  </si>
+  <si>
+    <t>Evolutionary Algorithms</t>
+  </si>
+  <si>
+    <t>Review languages for EAs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memetic Algorithms </t>
+  </si>
+  <si>
+    <t>Memetic Algorithms</t>
+  </si>
+  <si>
+    <t>Structure Sections</t>
+  </si>
+  <si>
+    <t>Bug Fixing 2</t>
   </si>
 </sst>
 </file>
@@ -280,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="180" wrapText="1"/>
@@ -300,6 +309,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,13 +587,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH41"/>
+  <dimension ref="A1:AH43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R18" sqref="R18"/>
+      <selection pane="bottomRight" activeCell="AH35" sqref="AH35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -754,185 +764,221 @@
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="8"/>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="AB7" s="8"/>
-      <c r="AC7" s="8"/>
-      <c r="AD7" s="8"/>
-      <c r="AE7" s="8"/>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="AB8" s="8"/>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="8"/>
+      <c r="AE8" s="8"/>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="12"/>
+        <v>32</v>
+      </c>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
+        <v>23</v>
+      </c>
+      <c r="H12" s="12"/>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="A13" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="11"/>
+        <v>33</v>
+      </c>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
+      <c r="A15" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H16" s="10"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
+        <v>19</v>
+      </c>
+      <c r="G16" s="11"/>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
+        <v>23</v>
+      </c>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="10"/>
+        <v>25</v>
+      </c>
+      <c r="H18" s="10"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
+        <v>26</v>
+      </c>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="T20" s="11"/>
-      <c r="U20" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="10"/>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
-      <c r="T21" s="10"/>
-      <c r="U21" s="10"/>
+      <c r="A21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="T22" s="10"/>
-      <c r="U22" s="10"/>
+      <c r="A22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="T22" s="11"/>
+      <c r="U22" s="11"/>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+        <v>34</v>
+      </c>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="11"/>
+      <c r="W23" s="11"/>
+      <c r="X23" s="11"/>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="10"/>
-      <c r="S24" s="10"/>
+        <v>36</v>
+      </c>
+      <c r="T24" s="10"/>
+      <c r="U24" s="10"/>
+      <c r="V24" s="10"/>
+      <c r="W24" s="10"/>
+      <c r="Y24" s="11"/>
+      <c r="Z24" s="11"/>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A25" s="6"/>
-      <c r="R25" s="10"/>
-      <c r="S25" s="10"/>
+      <c r="A25" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="T25" s="10"/>
+      <c r="U25" s="10"/>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
-        <v>11</v>
-      </c>
+      <c r="A26" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="9"/>
+        <v>27</v>
+      </c>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="10"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="9"/>
+      <c r="A28" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
+        <v>12</v>
+      </c>
+      <c r="B29" s="9"/>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="10"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R31" s="9"/>
+      <c r="S31" s="9"/>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="AB30" s="9"/>
-      <c r="AC30" s="9"/>
-      <c r="AD30" s="9"/>
-      <c r="AE30" s="9"/>
-    </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A31" s="6"/>
-    </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A32" s="6"/>
+      <c r="AB32" s="9"/>
+      <c r="AC32" s="9"/>
+      <c r="AD32" s="9"/>
+      <c r="AE32" s="9"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
@@ -960,6 +1006,12 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="6"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Attempted to add work plan to latex
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -26,39 +26,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Benjamin Joshua Charlton</author>
-  </authors>
-  <commentList>
-    <comment ref="A31" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Benjamin Joshua Charlton:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-Not counting in revision time 
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
@@ -199,15 +166,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="81"/>
+      <sz val="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="81"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -294,7 +263,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="180" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -310,6 +278,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,32 +557,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AH35" sqref="AH35"/>
+      <selection pane="bottomRight" sqref="A1:AH32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5" customWidth="1"/>
-    <col min="8" max="11" width="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="20" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="24" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="28" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="33" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="2" max="34" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" s="1" customFormat="1" ht="127" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -634,387 +597,388 @@
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="15">
         <v>43003</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="15">
         <v>43010</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="15">
         <v>43017</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="15">
         <v>43024</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="15">
         <v>43031</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="15">
         <v>43038</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="15">
         <v>43045</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="15">
         <v>43052</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="15">
         <v>43059</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="15">
         <v>43066</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="15">
         <v>43073</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="15">
         <v>43080</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="15">
         <v>43087</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="15">
         <v>43094</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="15">
         <v>43101</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2" s="15">
         <v>43108</v>
       </c>
-      <c r="R2" s="2">
+      <c r="R2" s="15">
         <v>43115</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="15">
         <v>43122</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2" s="15">
         <v>43129</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2" s="15">
         <v>43136</v>
       </c>
-      <c r="V2" s="2">
+      <c r="V2" s="15">
         <v>43143</v>
       </c>
-      <c r="W2" s="2">
+      <c r="W2" s="15">
         <v>43150</v>
       </c>
-      <c r="X2" s="2">
+      <c r="X2" s="15">
         <v>43157</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="Y2" s="15">
         <v>43164</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="Z2" s="15">
         <v>43171</v>
       </c>
-      <c r="AA2" s="2">
+      <c r="AA2" s="15">
         <v>43178</v>
       </c>
-      <c r="AB2" s="2">
+      <c r="AB2" s="15">
         <v>43185</v>
       </c>
-      <c r="AC2" s="2">
+      <c r="AC2" s="15">
         <v>43192</v>
       </c>
-      <c r="AD2" s="2">
+      <c r="AD2" s="15">
         <v>43199</v>
       </c>
-      <c r="AE2" s="2">
+      <c r="AE2" s="15">
         <v>43206</v>
       </c>
-      <c r="AF2" s="2">
+      <c r="AF2" s="15">
         <v>43213</v>
       </c>
-      <c r="AG2" s="2">
+      <c r="AG2" s="15">
         <v>43220</v>
       </c>
-      <c r="AH2" s="3"/>
+      <c r="AH2" s="2"/>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
-      <c r="V7" s="10"/>
-      <c r="W7" s="10"/>
-      <c r="X7" s="10"/>
-      <c r="Y7" s="10"/>
-      <c r="Z7" s="10"/>
-      <c r="AA7" s="8"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="7"/>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AB8" s="8"/>
-      <c r="AC8" s="8"/>
-      <c r="AD8" s="8"/>
-      <c r="AE8" s="8"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="12"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="12"/>
+      <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="12"/>
+      <c r="H12" s="11"/>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="14"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="13"/>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="11"/>
+      <c r="G16" s="10"/>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H18" s="10"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="10"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="9"/>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="T22" s="11"/>
-      <c r="U22" s="11"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="T23" s="10"/>
-      <c r="U23" s="10"/>
-      <c r="V23" s="11"/>
-      <c r="W23" s="11"/>
-      <c r="X23" s="11"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="10"/>
+      <c r="W23" s="10"/>
+      <c r="X23" s="10"/>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="T24" s="10"/>
-      <c r="U24" s="10"/>
-      <c r="V24" s="10"/>
-      <c r="W24" s="10"/>
-      <c r="Y24" s="11"/>
-      <c r="Z24" s="11"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
+      <c r="Y24" s="10"/>
+      <c r="Z24" s="10"/>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="T25" s="10"/>
-      <c r="U25" s="10"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="13"/>
-      <c r="R27" s="10"/>
-      <c r="S27" s="10"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="9"/>
+      <c r="B29" s="8"/>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="10"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="R31" s="9"/>
-      <c r="S31" s="9"/>
+      <c r="R31" s="8"/>
+      <c r="S31" s="8"/>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AB32" s="9"/>
-      <c r="AC32" s="9"/>
-      <c r="AD32" s="9"/>
-      <c r="AE32" s="9"/>
+      <c r="AB32" s="8"/>
+      <c r="AC32" s="8"/>
+      <c r="AD32" s="8"/>
+      <c r="AE32" s="8"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="6"/>
+      <c r="A33" s="5"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="6"/>
+      <c r="A34" s="5"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="6"/>
+      <c r="A35" s="5"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="6"/>
+      <c r="A36" s="5"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="6"/>
+      <c r="A37" s="5"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="6"/>
+      <c r="A38" s="5"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="6"/>
+      <c r="A39" s="5"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="6"/>
+      <c r="A40" s="5"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="6"/>
+      <c r="A41" s="5"/>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="6"/>
+      <c r="A42" s="5"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="6"/>
+      <c r="A43" s="5"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created the base GA structure
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Leafeon/Desktop/g53IDS/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Leafeon/Desktop/G53IDS/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5240" yWindow="-21160" windowWidth="38400" windowHeight="21160" tabRatio="500"/>
+    <workbookView xWindow="46780" yWindow="-8120" windowWidth="38400" windowHeight="21160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -564,7 +564,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" sqref="A1:AH32"/>
+      <selection pane="bottomRight" activeCell="V19" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated WorkPlan to latest version
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="46780" yWindow="-8120" windowWidth="38400" windowHeight="21160" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="440" windowWidth="34360" windowHeight="28360" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="Interim Report" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="43">
   <si>
     <t>Week</t>
   </si>
@@ -143,13 +144,32 @@
   </si>
   <si>
     <t>Bug Fixing 2</t>
+  </si>
+  <si>
+    <t>Run GA on Benchmark Function</t>
+  </si>
+  <si>
+    <t>Poké API</t>
+  </si>
+  <si>
+    <t>Demo</t>
+  </si>
+  <si>
+    <t>17/18th May
+Presentation and Demo</t>
+  </si>
+  <si>
+    <t>Finalise Presentation</t>
+  </si>
+  <si>
+    <t>Work on Presentation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -178,8 +198,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -216,8 +243,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD883FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -254,11 +287,76 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="180" wrapText="1"/>
@@ -281,12 +379,38 @@
     <xf numFmtId="16" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFD883FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -560,11 +684,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="V19" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="O21" sqref="O21:Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -981,4 +1105,599 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AJ70"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="AI30" sqref="AI30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="7.5" customWidth="1"/>
+    <col min="12" max="12" width="7.5" style="28" customWidth="1"/>
+    <col min="13" max="34" width="7.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" s="1" customFormat="1" ht="127" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="15">
+        <v>43003</v>
+      </c>
+      <c r="C2" s="15">
+        <v>43010</v>
+      </c>
+      <c r="D2" s="15">
+        <v>43017</v>
+      </c>
+      <c r="E2" s="15">
+        <v>43024</v>
+      </c>
+      <c r="F2" s="15">
+        <v>43031</v>
+      </c>
+      <c r="G2" s="15">
+        <v>43038</v>
+      </c>
+      <c r="H2" s="15">
+        <v>43045</v>
+      </c>
+      <c r="I2" s="15">
+        <v>43052</v>
+      </c>
+      <c r="J2" s="15">
+        <v>43059</v>
+      </c>
+      <c r="K2" s="15">
+        <v>43066</v>
+      </c>
+      <c r="L2" s="32">
+        <v>43073</v>
+      </c>
+      <c r="M2" s="15">
+        <v>43080</v>
+      </c>
+      <c r="N2" s="15">
+        <v>43087</v>
+      </c>
+      <c r="O2" s="15">
+        <v>43094</v>
+      </c>
+      <c r="P2" s="15">
+        <v>43101</v>
+      </c>
+      <c r="Q2" s="15">
+        <v>43108</v>
+      </c>
+      <c r="R2" s="15">
+        <v>43115</v>
+      </c>
+      <c r="S2" s="15">
+        <v>43122</v>
+      </c>
+      <c r="T2" s="15">
+        <v>43129</v>
+      </c>
+      <c r="U2" s="15">
+        <v>43136</v>
+      </c>
+      <c r="V2" s="15">
+        <v>43143</v>
+      </c>
+      <c r="W2" s="15">
+        <v>43150</v>
+      </c>
+      <c r="X2" s="15">
+        <v>43157</v>
+      </c>
+      <c r="Y2" s="15">
+        <v>43164</v>
+      </c>
+      <c r="Z2" s="15">
+        <v>43171</v>
+      </c>
+      <c r="AA2" s="15">
+        <v>43178</v>
+      </c>
+      <c r="AB2" s="15">
+        <v>43185</v>
+      </c>
+      <c r="AC2" s="15">
+        <v>43192</v>
+      </c>
+      <c r="AD2" s="15">
+        <v>43199</v>
+      </c>
+      <c r="AE2" s="15">
+        <v>43206</v>
+      </c>
+      <c r="AF2" s="15">
+        <v>43213</v>
+      </c>
+      <c r="AG2" s="15">
+        <v>43220</v>
+      </c>
+      <c r="AH2" s="15">
+        <v>43227</v>
+      </c>
+      <c r="AI2" s="15">
+        <v>43234</v>
+      </c>
+      <c r="AJ2" s="15">
+        <v>43241</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="L4" s="5"/>
+    </row>
+    <row r="5" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="7"/>
+      <c r="L5" s="5"/>
+    </row>
+    <row r="6" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="16"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="26"/>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="9"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="7"/>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="5"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" s="23"/>
+      <c r="L12" s="5"/>
+    </row>
+    <row r="13" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="23"/>
+      <c r="M13" s="23"/>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L14" s="5"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L15" s="5"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+    </row>
+    <row r="16" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="28"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="20"/>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="9"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="22"/>
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" s="9"/>
+      <c r="J19" s="19"/>
+      <c r="M19" s="20"/>
+    </row>
+    <row r="20" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I20" s="9"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="22"/>
+    </row>
+    <row r="21" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="27"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="22"/>
+      <c r="Q21" s="24"/>
+    </row>
+    <row r="22" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="Q22" s="30"/>
+      <c r="S22" s="19"/>
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="29"/>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L24" s="5"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="10"/>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L25" s="5"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="10"/>
+      <c r="W25" s="10"/>
+      <c r="X25" s="10"/>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L26" s="5"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
+      <c r="W26" s="9"/>
+      <c r="Y26" s="10"/>
+      <c r="Z26" s="10"/>
+    </row>
+    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L27" s="5"/>
+      <c r="T27" s="9"/>
+      <c r="U27" s="9"/>
+    </row>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L28" s="5"/>
+      <c r="AG28" s="31"/>
+      <c r="AH28" s="31"/>
+    </row>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L29" s="5"/>
+      <c r="AI29" s="31"/>
+    </row>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L30" s="5"/>
+    </row>
+    <row r="31" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="L31" s="5"/>
+    </row>
+    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L32" s="5"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="12"/>
+      <c r="R32" s="9"/>
+      <c r="S32" s="9"/>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L33" s="5"/>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="L34" s="5"/>
+    </row>
+    <row r="35" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="9"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35" s="5"/>
+      <c r="M35"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="8"/>
+      <c r="R35"/>
+      <c r="S35"/>
+      <c r="T35"/>
+      <c r="U35"/>
+      <c r="V35"/>
+      <c r="W35"/>
+      <c r="X35"/>
+      <c r="Y35"/>
+      <c r="Z35"/>
+      <c r="AA35"/>
+      <c r="AB35"/>
+      <c r="AC35"/>
+      <c r="AD35"/>
+      <c r="AE35"/>
+    </row>
+    <row r="36" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36" s="5"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="R36" s="8"/>
+      <c r="S36" s="8"/>
+      <c r="T36"/>
+      <c r="U36"/>
+      <c r="V36"/>
+      <c r="W36"/>
+      <c r="X36"/>
+      <c r="Y36"/>
+      <c r="Z36"/>
+      <c r="AA36"/>
+      <c r="AB36"/>
+      <c r="AC36"/>
+      <c r="AD36"/>
+      <c r="AE36"/>
+    </row>
+    <row r="37" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37"/>
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37" s="5"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
+      <c r="R37"/>
+      <c r="S37"/>
+      <c r="T37"/>
+      <c r="U37"/>
+      <c r="V37"/>
+      <c r="W37"/>
+      <c r="X37"/>
+      <c r="Y37"/>
+      <c r="Z37"/>
+      <c r="AA37"/>
+      <c r="AB37" s="8"/>
+      <c r="AC37" s="8"/>
+      <c r="AD37" s="8"/>
+      <c r="AE37" s="8"/>
+    </row>
+    <row r="38" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="55" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="56" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="57" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="58" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="59" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="60" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="61" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="62" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="63" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="64" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="65" spans="1:1" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="66" spans="1:1" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="67" spans="1:1" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" s="28"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="28"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the work plan
</commit_message>
<xml_diff>
--- a/Documentation/WorkPlan.xlsx
+++ b/Documentation/WorkPlan.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="440" windowWidth="34360" windowHeight="28360" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="80" yWindow="440" windowWidth="68720" windowHeight="28360" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="Interim Report" sheetId="3" r:id="rId2"/>
+    <sheet name="Dissertation" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="45">
   <si>
     <t>Week</t>
   </si>
@@ -163,6 +164,12 @@
   </si>
   <si>
     <t>Work on Presentation</t>
+  </si>
+  <si>
+    <t>Running of Final Code</t>
+  </si>
+  <si>
+    <t>G53DIA Coursework</t>
   </si>
 </sst>
 </file>
@@ -250,7 +257,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -352,11 +359,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="180" wrapText="1"/>
@@ -398,6 +416,19 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1111,11 +1142,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AI30" sqref="AI30"/>
+      <selection pane="bottomRight" activeCell="Y26" sqref="Y26:Z26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1700,4 +1731,700 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AL70"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="N39" sqref="N39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31.83203125" customWidth="1"/>
+    <col min="2" max="11" width="9.1640625" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="28" customWidth="1"/>
+    <col min="13" max="35" width="9.1640625" customWidth="1"/>
+    <col min="36" max="36" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" s="1" customFormat="1" ht="127" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40"/>
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
+      <c r="AC1" s="40"/>
+      <c r="AD1" s="40"/>
+      <c r="AE1" s="40"/>
+      <c r="AF1" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG1" s="40"/>
+      <c r="AH1" s="40"/>
+      <c r="AI1" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ1" s="40"/>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="15">
+        <v>43003</v>
+      </c>
+      <c r="C2" s="15">
+        <v>43010</v>
+      </c>
+      <c r="D2" s="15">
+        <v>43017</v>
+      </c>
+      <c r="E2" s="15">
+        <v>43024</v>
+      </c>
+      <c r="F2" s="15">
+        <v>43031</v>
+      </c>
+      <c r="G2" s="15">
+        <v>43038</v>
+      </c>
+      <c r="H2" s="15">
+        <v>43045</v>
+      </c>
+      <c r="I2" s="15">
+        <v>43052</v>
+      </c>
+      <c r="J2" s="15">
+        <v>43059</v>
+      </c>
+      <c r="K2" s="15">
+        <v>43066</v>
+      </c>
+      <c r="L2" s="41">
+        <v>43073</v>
+      </c>
+      <c r="M2" s="15">
+        <v>43080</v>
+      </c>
+      <c r="N2" s="15">
+        <v>43087</v>
+      </c>
+      <c r="O2" s="15">
+        <v>43094</v>
+      </c>
+      <c r="P2" s="15">
+        <v>43101</v>
+      </c>
+      <c r="Q2" s="15">
+        <v>43108</v>
+      </c>
+      <c r="R2" s="15">
+        <v>43115</v>
+      </c>
+      <c r="S2" s="15">
+        <v>43122</v>
+      </c>
+      <c r="T2" s="15">
+        <v>43129</v>
+      </c>
+      <c r="U2" s="15">
+        <v>43136</v>
+      </c>
+      <c r="V2" s="15">
+        <v>43143</v>
+      </c>
+      <c r="W2" s="15">
+        <v>43150</v>
+      </c>
+      <c r="X2" s="15">
+        <v>43157</v>
+      </c>
+      <c r="Y2" s="15">
+        <v>43164</v>
+      </c>
+      <c r="Z2" s="15">
+        <v>43171</v>
+      </c>
+      <c r="AA2" s="15">
+        <v>43178</v>
+      </c>
+      <c r="AB2" s="15">
+        <v>43185</v>
+      </c>
+      <c r="AC2" s="15">
+        <v>43192</v>
+      </c>
+      <c r="AD2" s="15">
+        <v>43199</v>
+      </c>
+      <c r="AE2" s="15">
+        <v>43206</v>
+      </c>
+      <c r="AF2" s="41">
+        <v>43213</v>
+      </c>
+      <c r="AG2" s="15">
+        <v>43220</v>
+      </c>
+      <c r="AH2" s="15">
+        <v>43227</v>
+      </c>
+      <c r="AI2" s="15">
+        <v>43234</v>
+      </c>
+      <c r="AJ2" s="15"/>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="5"/>
+      <c r="AF3" s="5"/>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="L4" s="5"/>
+      <c r="AF4" s="5"/>
+    </row>
+    <row r="5" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="7"/>
+      <c r="L5" s="5"/>
+      <c r="AF5" s="5"/>
+    </row>
+    <row r="6" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="16"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="26"/>
+      <c r="AF6" s="5"/>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="9"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="7"/>
+      <c r="AF7" s="5"/>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="5"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="5"/>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="5"/>
+      <c r="AF9" s="5"/>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="L10" s="5"/>
+      <c r="AF10" s="5"/>
+    </row>
+    <row r="11" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="L11" s="5"/>
+      <c r="AF11" s="5"/>
+    </row>
+    <row r="12" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" s="23"/>
+      <c r="L12" s="5"/>
+      <c r="AF12" s="5"/>
+    </row>
+    <row r="13" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="AF13" s="5"/>
+    </row>
+    <row r="14" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L14" s="5"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="X14" s="23"/>
+      <c r="AF14" s="5"/>
+    </row>
+    <row r="15" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L15" s="5"/>
+      <c r="AF15" s="5"/>
+    </row>
+    <row r="16" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="20"/>
+      <c r="L16" s="5"/>
+      <c r="AF16" s="5"/>
+    </row>
+    <row r="17" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="9"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="22"/>
+      <c r="L17" s="5"/>
+      <c r="AF17" s="5"/>
+    </row>
+    <row r="18" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="9"/>
+      <c r="J18" s="19"/>
+      <c r="M18" s="20"/>
+      <c r="AF18" s="5"/>
+    </row>
+    <row r="19" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" s="9"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="22"/>
+      <c r="AF19" s="5"/>
+    </row>
+    <row r="20" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="27"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="24"/>
+      <c r="AF20" s="5"/>
+    </row>
+    <row r="21" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="Q21" s="30"/>
+      <c r="S21" s="21"/>
+      <c r="T21" s="33"/>
+      <c r="U21" s="22"/>
+      <c r="AF21" s="5"/>
+    </row>
+    <row r="22" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="29"/>
+      <c r="Q22" s="29"/>
+      <c r="AF22" s="5"/>
+    </row>
+    <row r="23" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L23" s="5"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="9"/>
+      <c r="Y23" s="21"/>
+      <c r="Z23" s="38"/>
+      <c r="AF23" s="5"/>
+    </row>
+    <row r="24" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L24" s="5"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
+      <c r="Y24" s="24"/>
+      <c r="Z24" s="21"/>
+      <c r="AA24" s="22"/>
+      <c r="AB24" s="9"/>
+      <c r="AC24" s="9"/>
+      <c r="AF24" s="5"/>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L25" s="5"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="AF25" s="5"/>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L26" s="5"/>
+      <c r="AF26" s="5"/>
+      <c r="AG26" s="31"/>
+      <c r="AH26" s="31"/>
+    </row>
+    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L27" s="5"/>
+      <c r="AF27" s="5"/>
+      <c r="AI27" s="31"/>
+    </row>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L28" s="5"/>
+      <c r="AF28" s="5"/>
+    </row>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="L29" s="5"/>
+      <c r="AF29" s="5"/>
+    </row>
+    <row r="30" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L30" s="5"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="9"/>
+      <c r="S30" s="9"/>
+      <c r="AF30" s="5"/>
+    </row>
+    <row r="31" spans="1:35" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="L31" s="5"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
+      <c r="S31" s="9"/>
+      <c r="AB31" s="34"/>
+      <c r="AC31" s="35"/>
+      <c r="AF31" s="5"/>
+    </row>
+    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L32" s="5"/>
+      <c r="AF32" s="5"/>
+    </row>
+    <row r="33" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="L33" s="5"/>
+      <c r="AF33" s="5"/>
+    </row>
+    <row r="34" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="9"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34" s="5"/>
+      <c r="M34"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="R34"/>
+      <c r="S34"/>
+      <c r="T34"/>
+      <c r="U34"/>
+      <c r="V34"/>
+      <c r="W34"/>
+      <c r="X34"/>
+      <c r="Y34"/>
+      <c r="Z34"/>
+      <c r="AA34"/>
+      <c r="AB34"/>
+      <c r="AC34"/>
+      <c r="AD34"/>
+      <c r="AE34"/>
+      <c r="AF34" s="5"/>
+      <c r="AL34" s="39"/>
+    </row>
+    <row r="35" spans="1:38" s="28" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35" s="5"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+      <c r="R35" s="8"/>
+      <c r="S35" s="8"/>
+      <c r="T35"/>
+      <c r="U35"/>
+      <c r="V35"/>
+      <c r="W35"/>
+      <c r="X35"/>
+      <c r="Y35"/>
+      <c r="Z35"/>
+      <c r="AA35"/>
+      <c r="AB35"/>
+      <c r="AC35"/>
+      <c r="AD35"/>
+      <c r="AE35"/>
+      <c r="AF35" s="5"/>
+    </row>
+    <row r="36" spans="1:38" s="28" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36" s="5"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="R36" s="9"/>
+      <c r="S36" s="9"/>
+      <c r="T36"/>
+      <c r="U36"/>
+      <c r="V36" s="36"/>
+      <c r="W36" s="37"/>
+      <c r="X36"/>
+      <c r="Y36"/>
+      <c r="Z36"/>
+      <c r="AA36" s="36"/>
+      <c r="AB36" s="37"/>
+      <c r="AC36"/>
+      <c r="AD36"/>
+      <c r="AE36"/>
+      <c r="AF36" s="5"/>
+    </row>
+    <row r="37" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37"/>
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37" s="5"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
+      <c r="R37"/>
+      <c r="S37"/>
+      <c r="T37"/>
+      <c r="U37"/>
+      <c r="V37"/>
+      <c r="W37"/>
+      <c r="X37"/>
+      <c r="Y37"/>
+      <c r="Z37"/>
+      <c r="AA37"/>
+      <c r="AB37" s="8"/>
+      <c r="AC37" s="8"/>
+      <c r="AD37" s="8"/>
+      <c r="AE37" s="8"/>
+      <c r="AF37" s="5"/>
+    </row>
+    <row r="38" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:38" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="55" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="56" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="57" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="58" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="59" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="60" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="61" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="62" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="63" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="64" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="65" spans="1:1" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="66" spans="1:1" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="67" spans="1:1" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" s="28"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="28"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>